<commit_message>
updated clockCalculations.xlsx to show ticks/second
</commit_message>
<xml_diff>
--- a/Documents/clockCalculations.xlsx
+++ b/Documents/clockCalculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>MHz</t>
   </si>
@@ -36,10 +36,19 @@
     <t>ns</t>
   </si>
   <si>
-    <t>resolution</t>
-  </si>
-  <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>bit resolution</t>
+  </si>
+  <si>
+    <t>clock speed</t>
+  </si>
+  <si>
+    <t>length of clock tick</t>
+  </si>
+  <si>
+    <t>ticks/sec</t>
   </si>
 </sst>
 </file>
@@ -371,124 +380,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="str">
+        <f>"-&gt;"</f>
+        <v>-&gt;</v>
+      </c>
+      <c r="F1">
         <f>10*10^6</f>
         <v>10000000</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2">
-        <f>CONVERT(A1*D4,"sec",B2)</f>
+        <f>CONVERT(A1*F4,"sec",B2)</f>
         <v>5.0903316100740739</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <f>D1^-1</f>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E4" si="0">"-&gt;"</f>
+        <v>-&gt;</v>
+      </c>
+      <c r="F2">
+        <f>F1^-1</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>1</v>
-      </c>
-      <c r="F2">
-        <f>D2*1000</f>
-        <v>9.9999999999999991E-5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
       </c>
       <c r="H2">
         <f>F2*1000</f>
-        <v>9.9999999999999992E-2</v>
+        <v>9.9999999999999991E-5</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2">
         <f>H2*1000</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <f>J2*1000</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="D3">
+    <row r="3" spans="1:13">
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>-&gt;</v>
+      </c>
+      <c r="F3">
         <v>1024</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4">
         <f>2^16</f>
         <v>65536</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <f>D2*D3</f>
+        <v>7</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>-&gt;</v>
+      </c>
+      <c r="F4">
+        <f>F2*F3</f>
         <v>1.024E-4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>1</v>
-      </c>
-      <c r="F4">
-        <f>D4*1000</f>
-        <v>0.10239999999999999</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
       </c>
       <c r="H4">
         <f>F4*1000</f>
-        <v>102.39999999999999</v>
+        <v>0.10239999999999999</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <f>H4*1000</f>
+        <v>102.39999999999999</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <f>J4*1000</f>
         <v>102399.99999999999</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5">
-        <f>CONVERT(A4*D4,"sec",B5)</f>
+        <f>CONVERT(A4*F4,"sec",B5)</f>
         <v>6.7108863999999997</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
+      </c>
+      <c r="F5">
+        <f>1/F4</f>
+        <v>9765.625</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>